<commit_message>
modifiche al documento excel
</commit_message>
<xml_diff>
--- a/progressi_palestra.xlsx
+++ b/progressi_palestra.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>mese</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>giorni settembre</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -114,6 +117,9 @@
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -432,12 +438,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -547,7 +553,9 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="E9" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
correzioni varie e inserimento valori nelle celle
</commit_message>
<xml_diff>
--- a/progressi_palestra.xlsx
+++ b/progressi_palestra.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>mese</t>
   </si>
@@ -35,6 +35,21 @@
   </si>
   <si>
     <t>giorni settembre</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>km fatti</t>
+  </si>
+  <si>
+    <t>alexboy15</t>
+  </si>
+  <si>
+    <t>xmoro</t>
+  </si>
+  <si>
+    <t>freshcanta</t>
   </si>
 </sst>
 </file>
@@ -60,7 +75,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -92,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -121,11 +136,14 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -438,12 +456,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -528,8 +546,12 @@
         <v>75.2</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="F7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -552,8 +574,12 @@
         <v>74.85</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="10">
+        <v>8</v>
+      </c>
       <c r="F9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -564,8 +590,12 @@
         <v>74.35</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="10">
+        <v>9</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -576,8 +606,12 @@
         <v>74.35</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="10">
+        <v>4</v>
+      </c>
       <c r="F11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
aggiunte due colonne E9 e F9
</commit_message>
<xml_diff>
--- a/progressi_palestra.xlsx
+++ b/progressi_palestra.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>mese</t>
   </si>
@@ -53,6 +53,30 @@
   </si>
   <si>
     <t>freshcanta</t>
+  </si>
+  <si>
+    <t>somatotipo</t>
+  </si>
+  <si>
+    <t>dieta</t>
+  </si>
+  <si>
+    <t>endomorfo</t>
+  </si>
+  <si>
+    <t>carboidrati</t>
+  </si>
+  <si>
+    <t>mesomorfo</t>
+  </si>
+  <si>
+    <t>proteine</t>
+  </si>
+  <si>
+    <t>ectomorfo</t>
+  </si>
+  <si>
+    <t>zuccheri</t>
   </si>
 </sst>
 </file>
@@ -711,8 +735,12 @@
       <c r="B15" s="7"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="G15" s="3"/>
       <c r="H15" s="5"/>
     </row>
@@ -723,8 +751,12 @@
       <c r="D16" s="14">
         <f>8+9</f>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
+      <c r="E16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G16" s="3"/>
       <c r="H16" s="5"/>
     </row>
@@ -733,8 +765,12 @@
       <c r="B17" s="7"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
+      <c r="E17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G17" s="3"/>
       <c r="H17" s="5"/>
     </row>
@@ -743,8 +779,12 @@
       <c r="B18" s="7"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="4"/>
+      <c r="E18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G18" s="3"/>
       <c r="H18" s="5"/>
     </row>

</xml_diff>